<commit_message>
Update modal build to handle PDF, YouTube
</commit_message>
<xml_diff>
--- a/rondo.xlsx
+++ b/rondo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashwanth/Documents/Yashu/San Jose/DHC/Original_Rondo_repo/rondo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/012768353/Git/rondo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7121FCB-8210-9D4C-82ED-4DB084F8C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC10232-A06A-024B-B992-95F9C0D33100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35720" yWindow="-4640" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="211">
   <si>
     <t>Title</t>
   </si>
@@ -1091,6 +1091,9 @@
   </si>
   <si>
     <t>Pioneers </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RUUDx1noGB8</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1451,9 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -2195,7 +2200,9 @@
         <v>134</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>210</v>
+      </c>
       <c r="J21" s="6" t="s">
         <v>135</v>
       </c>
@@ -11443,8 +11450,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>